<commit_message>
Working on weight forms.
</commit_message>
<xml_diff>
--- a/data_challenge/cross trials.xlsx
+++ b/data_challenge/cross trials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12660" yWindow="0" windowWidth="15480" windowHeight="17460" tabRatio="611" activeTab="5"/>
+    <workbookView xWindow="12660" yWindow="0" windowWidth="15480" windowHeight="17460" tabRatio="611" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="22">
   <si>
     <t>Crosses:</t>
   </si>
@@ -143,8 +143,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -176,7 +182,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -189,6 +195,9 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -201,6 +210,9 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1275,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1348,27 +1360,59 @@
         <v>12.38026</v>
       </c>
     </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>15484016</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>75000000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>0.20645354666666599</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>12.3872128</v>
+      </c>
+    </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>6</v>
       </c>
       <c r="B24">
         <f>SUM(B1:B22)</f>
-        <v>2476270</v>
+        <v>17960286</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="2">
         <f>SUM(D1:D21)</f>
-        <v>12000000</v>
+        <v>87000000</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="1">
         <f>B24/D24</f>
-        <v>0.20635583333333332</v>
+        <v>0.20644006896551725</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -1406,8 +1450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1511,27 +1555,91 @@
         <v>4.5391263333333303</v>
       </c>
     </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>34047452</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>75000000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>0.45396602666666602</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>4.5396602666666599</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>34053806</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>75000000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>0.45405074666666601</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>4.5405074666666598</v>
+      </c>
+    </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>6</v>
       </c>
       <c r="B24">
         <f>SUM(B1:B22)</f>
-        <v>30642113</v>
+        <v>98743371</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="2">
         <f>SUM(D1:D21)</f>
-        <v>67500000</v>
+        <v>217500000</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="1">
         <f>B24/D24</f>
-        <v>0.45395722962962964</v>
+        <v>0.45399251034482757</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -1556,6 +1664,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>